<commit_message>
Commit Create Cancel Rebill File
</commit_message>
<xml_diff>
--- a/regression-tests/src/test/java/com/hansencx/portal/datatest/Create Cancel Rebill - Filled In Template.xlsx
+++ b/regression-tests/src/test/java/com/hansencx/portal/datatest/Create Cancel Rebill - Filled In Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trinhh\OneDrive - Hansen Technologies Limited\Billing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trinhh\OneDrive - Hansen Technologies Limited\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{775B25FF-A7D9-4C0D-BDF3-E4B3871BA876}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{661DF12C-61BE-4D5C-80BE-F2903277796D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27690" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>KY_PND_SEQ_TRANS</t>
   </si>
@@ -55,7 +55,7 @@
     <t>WinkelJ</t>
   </si>
   <si>
-    <t>QA automation test</t>
+    <t>QA automation test same supplier</t>
   </si>
 </sst>
 </file>
@@ -432,22 +432,22 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -470,9 +470,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>56669823</v>
+        <v>63098612</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -493,13 +493,28 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>61838590</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>